<commit_message>
Updated currency units and new wedge diagram excl LULUCF
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E145C7-DA32-48E1-AEFA-9C38A9EDE413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B35506-C083-4DF5-9DF7-5DD16A38E814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,22 +105,22 @@
     <t>Recall, this variable is "dollars per large/medium/small currency output unit"</t>
   </si>
   <si>
-    <t>2019 dollars per 2012 dollar</t>
-  </si>
-  <si>
-    <t>2020 dollars</t>
-  </si>
-  <si>
-    <t>million 2020 dollars</t>
-  </si>
-  <si>
-    <t>billion 2020 dollars</t>
-  </si>
-  <si>
-    <t>which in this case is "2012 dollars per 2020 dollar."</t>
-  </si>
-  <si>
     <t>2012 dollars are worth more than 2020 dollars, so we need a</t>
+  </si>
+  <si>
+    <t>billion 2021 dollars</t>
+  </si>
+  <si>
+    <t>million 2021 dollars</t>
+  </si>
+  <si>
+    <t>2021 dollars</t>
+  </si>
+  <si>
+    <t>2012 dollars per 2021 dollars</t>
+  </si>
+  <si>
+    <t>which in this case is "2012 dollars per 2021 dollar."</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -624,15 +624,16 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.88711067149387013</v>
+        <f>1/1.21</f>
+        <v>0.82644628099173556</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,12 +643,12 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,7 +697,7 @@
       </c>
       <c r="B2" s="3">
         <f>10^9*About!$A$26</f>
-        <v>887110671.49387014</v>
+        <v>826446280.99173558</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +730,7 @@
       </c>
       <c r="B2" s="8">
         <f>10^6*About!$A$26</f>
-        <v>887110.67149387009</v>
+        <v>826446.28099173552</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +763,7 @@
       </c>
       <c r="B2" s="7">
         <f>1*About!A26</f>
-        <v>0.88711067149387013</v>
+        <v>0.82644628099173556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>